<commit_message>
File detection cleanup. Made types game specfic. Added making textures opaque, to show certain textures that are all transparent, like GenZ makeup
</commit_message>
<xml_diff>
--- a/docs/adfb.xlsx
+++ b/docs/adfb.xlsx
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="137">
+  <si>
+    <t xml:space="preserve">GZB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP</t>
+  </si>
   <si>
     <t xml:space="preserve">ADF_BARE</t>
   </si>
@@ -440,6 +446,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -457,12 +464,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -505,7 +518,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -514,7 +527,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -571,7 +588,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -595,10 +612,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:K114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I62" activeCellId="0" sqref="I62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -607,32 +624,12 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
-        <v>43486</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>39.316517</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="I1" s="0" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,22 +643,28 @@
         <v>18</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>39.319219</v>
+        <v>39.316517</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,22 +678,28 @@
         <v>18</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>39.3208</v>
+        <v>39.319219</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,22 +713,28 @@
         <v>18</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>39.320913</v>
+        <v>39.3208</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,22 +748,28 @@
         <v>18</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>39.322027</v>
+        <v>39.320913</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,22 +783,28 @@
         <v>18</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>39.322668</v>
+        <v>39.322027</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,22 +818,28 @@
         <v>18</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>39.324859</v>
+        <v>39.322668</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,22 +853,28 @@
         <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>39.327766</v>
+        <v>39.324859</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,22 +888,28 @@
         <v>18</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>39.327901</v>
+        <v>39.327766</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,22 +923,28 @@
         <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>39.329947</v>
+        <v>39.327901</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,22 +958,28 @@
         <v>18</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>39.330808</v>
+        <v>39.329947</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,22 +993,28 @@
         <v>18</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>39.334652</v>
+        <v>39.330808</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,22 +1028,28 @@
         <v>18</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>39.335889</v>
+        <v>39.334652</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,22 +1063,28 @@
         <v>18</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>39.336201</v>
+        <v>39.335889</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,22 +1098,28 @@
         <v>18</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>39.336416</v>
+        <v>39.336201</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,22 +1133,28 @@
         <v>18</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>39.336525</v>
+        <v>39.336416</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,21 +1168,27 @@
         <v>18</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>39.314237</v>
+        <v>39.336525</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="0" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1110,22 +1203,24 @@
         <v>18</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>39.31596</v>
+        <v>39.314237</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,22 +1234,24 @@
         <v>18</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>39.318884</v>
+        <v>39.31596</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,22 +1265,24 @@
         <v>18</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>39.319769</v>
+        <v>39.318884</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1197,22 +1296,24 @@
         <v>18</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>39.322551</v>
+        <v>39.319769</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>25</v>
+        <v>4</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,22 +1327,24 @@
         <v>18</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>39.323162</v>
+        <v>39.322551</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,22 +1358,24 @@
         <v>18</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>39.325702</v>
+        <v>39.323162</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>27</v>
+        <v>4</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1284,22 +1389,24 @@
         <v>18</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>39.329641</v>
+        <v>39.325702</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>28</v>
+        <v>4</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,22 +1420,24 @@
         <v>18</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>39.330069</v>
+        <v>39.329641</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>29</v>
+        <v>4</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,22 +1451,24 @@
         <v>18</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>39.330197</v>
+        <v>39.330069</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1371,22 +1482,24 @@
         <v>18</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>39.330657</v>
+        <v>39.330197</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1400,22 +1513,24 @@
         <v>18</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>39.333622</v>
+        <v>39.330657</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>32</v>
+        <v>4</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,21 +1544,23 @@
         <v>18</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>39.318033</v>
+        <v>39.333622</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="0" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1458,22 +1575,24 @@
         <v>18</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>39.323603</v>
+        <v>39.318033</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I30" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,22 +1606,24 @@
         <v>18</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>39.335472</v>
+        <v>39.323603</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>36</v>
+        <v>4</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,21 +1637,23 @@
         <v>18</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>39.328033</v>
+        <v>39.335472</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="I32" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="0" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1545,21 +1668,24 @@
         <v>18</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>39.326327</v>
+        <v>39.328033</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H33" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="I33" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" s="0" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1574,21 +1700,24 @@
         <v>18</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>39.314074</v>
+        <v>39.326327</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="I34" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" s="0" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1603,22 +1732,25 @@
         <v>18</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>39.317098</v>
+        <v>39.314074</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I35" s="0" t="s">
         <v>43</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,22 +1764,25 @@
         <v>18</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>39.319013</v>
+        <v>39.317098</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1661,22 +1796,25 @@
         <v>18</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>39.320332</v>
+        <v>39.319013</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="J37" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,22 +1828,25 @@
         <v>18</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>39.320466</v>
+        <v>39.320332</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="J38" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,22 +1860,25 @@
         <v>18</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>39.320593</v>
+        <v>39.320466</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="J39" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,22 +1892,25 @@
         <v>18</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>39.321183</v>
+        <v>39.320593</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1777,22 +1924,25 @@
         <v>18</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>39.321762</v>
+        <v>39.321183</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,22 +1956,25 @@
         <v>18</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>39.322213</v>
+        <v>39.321762</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1835,22 +1988,25 @@
         <v>18</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>39.322341</v>
+        <v>39.322213</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>51</v>
+        <v>43</v>
+      </c>
+      <c r="J43" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,22 +2020,25 @@
         <v>18</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>39.323352</v>
+        <v>39.322341</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,22 +2052,25 @@
         <v>18</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>39.324125</v>
+        <v>39.323352</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>53</v>
+        <v>43</v>
+      </c>
+      <c r="J45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1922,22 +2084,25 @@
         <v>18</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>39.324254</v>
+        <v>39.324125</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>54</v>
+        <v>43</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,22 +2116,25 @@
         <v>18</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>39.325046</v>
+        <v>39.324254</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I47" s="0" t="s">
-        <v>55</v>
+        <v>43</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K47" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,22 +2148,25 @@
         <v>18</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>39.3253</v>
+        <v>39.325046</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I48" s="0" t="s">
-        <v>56</v>
+        <v>43</v>
+      </c>
+      <c r="J48" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,22 +2180,25 @@
         <v>18</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>39.326511</v>
+        <v>39.3253</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K49" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,22 +2212,25 @@
         <v>18</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>39.327339</v>
+        <v>39.326511</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I50" s="0" t="s">
-        <v>58</v>
+        <v>43</v>
+      </c>
+      <c r="J50" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,22 +2244,25 @@
         <v>18</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>39.327491</v>
+        <v>39.327339</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I51" s="0" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K51" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,22 +2276,25 @@
         <v>18</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>39.331081</v>
+        <v>39.327491</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>60</v>
+        <v>43</v>
+      </c>
+      <c r="J52" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K52" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2125,22 +2308,25 @@
         <v>18</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>39.333824</v>
+        <v>39.331081</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>61</v>
+        <v>43</v>
+      </c>
+      <c r="J53" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2154,22 +2340,25 @@
         <v>18</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>39.333964</v>
+        <v>39.333824</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>62</v>
+        <v>43</v>
+      </c>
+      <c r="J54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2183,22 +2372,25 @@
         <v>18</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>39.334798</v>
+        <v>39.333964</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I55" s="0" t="s">
-        <v>63</v>
+        <v>43</v>
+      </c>
+      <c r="J55" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,21 +2404,24 @@
         <v>18</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>39.331766</v>
+        <v>39.334798</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="I56" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J56" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K56" s="0" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2241,21 +2436,24 @@
         <v>18</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>39.328855</v>
+        <v>39.331766</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H57" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I57" s="0" t="s">
+      <c r="J57" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" s="0" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2270,22 +2468,25 @@
         <v>18</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>39.334234</v>
+        <v>39.328855</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I58" s="0" t="s">
         <v>68</v>
+      </c>
+      <c r="J58" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2299,22 +2500,25 @@
         <v>18</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>39.33449</v>
+        <v>39.334234</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I59" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="J59" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2328,22 +2532,25 @@
         <v>18</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>39.33532</v>
+        <v>39.33449</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="J60" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2357,21 +2564,24 @@
         <v>18</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>39.33033</v>
+        <v>39.33532</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I61" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J61" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K61" s="0" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2386,21 +2596,23 @@
         <v>18</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>39.318161</v>
+        <v>39.33033</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I62" s="0" t="s">
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="0" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2415,22 +2627,24 @@
         <v>18</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>39.324667</v>
+        <v>39.318161</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I63" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" s="3" t="s">
         <v>75</v>
+      </c>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2444,22 +2658,24 @@
         <v>18</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>39.326126</v>
+        <v>39.324667</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>76</v>
+        <v>4</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,22 +2689,24 @@
         <v>18</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>39.328284</v>
+        <v>39.326126</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I65" s="0" t="s">
-        <v>77</v>
+        <v>4</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,22 +2720,24 @@
         <v>18</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>39.33349</v>
+        <v>39.328284</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>78</v>
+        <v>4</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2531,22 +2751,24 @@
         <v>18</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>39.33601</v>
+        <v>39.33349</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I67" s="0" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,21 +2782,23 @@
         <v>18</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>39.32348</v>
+        <v>39.33601</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H68" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I68" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="0" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2589,22 +2813,25 @@
         <v>18</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>39.325818</v>
+        <v>39.32348</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I69" s="0" t="s">
         <v>82</v>
+      </c>
+      <c r="J69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K69" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2618,22 +2845,25 @@
         <v>18</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>39.326636</v>
+        <v>39.325818</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I70" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K70" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2647,22 +2877,25 @@
         <v>18</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>39.329414</v>
+        <v>39.326636</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I71" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="J71" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K71" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2676,22 +2909,25 @@
         <v>18</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>39.334101</v>
+        <v>39.329414</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I72" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="J72" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K72" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,21 +2941,24 @@
         <v>18</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>39.317296</v>
+        <v>39.334101</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I73" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H73" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K73" s="0" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2734,21 +2973,23 @@
         <v>18</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>39.336311</v>
+        <v>39.317296</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H74" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H74" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="I74" s="0" t="s">
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="0" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2763,21 +3004,23 @@
         <v>18</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>39.316071</v>
+        <v>39.336311</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H75" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H75" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I75" s="0" t="s">
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="0" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2792,21 +3035,23 @@
         <v>18</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>39.316256</v>
+        <v>39.316071</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H76" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H76" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I76" s="0" t="s">
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="0" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2821,22 +3066,24 @@
         <v>18</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>39.316373</v>
+        <v>39.316256</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I77" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H77" s="3" t="s">
         <v>94</v>
+      </c>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2850,22 +3097,24 @@
         <v>18</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>39.316807</v>
+        <v>39.316373</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I78" s="0" t="s">
-        <v>95</v>
+        <v>4</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2879,22 +3128,24 @@
         <v>18</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>39.316991</v>
+        <v>39.316807</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I79" s="0" t="s">
-        <v>96</v>
+        <v>4</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,22 +3159,24 @@
         <v>18</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>39.317389</v>
+        <v>39.316991</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I80" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2937,22 +3190,24 @@
         <v>18</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>39.317747</v>
+        <v>39.317389</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I81" s="0" t="s">
-        <v>98</v>
+        <v>4</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,22 +3221,24 @@
         <v>18</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>39.318522</v>
+        <v>39.317747</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I82" s="0" t="s">
-        <v>99</v>
+        <v>4</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,22 +3252,24 @@
         <v>18</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>39.320063</v>
+        <v>39.318522</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I83" s="0" t="s">
-        <v>100</v>
+        <v>4</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3024,22 +3283,24 @@
         <v>18</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>39.3202</v>
+        <v>39.320063</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I84" s="0" t="s">
-        <v>101</v>
+        <v>4</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,22 +3314,24 @@
         <v>18</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>39.321311</v>
+        <v>39.3202</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I85" s="0" t="s">
-        <v>102</v>
+        <v>4</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3082,22 +3345,24 @@
         <v>18</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>39.321639</v>
+        <v>39.321311</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I86" s="0" t="s">
-        <v>103</v>
+        <v>4</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3111,22 +3376,24 @@
         <v>18</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>39.322777</v>
+        <v>39.321639</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I87" s="0" t="s">
-        <v>104</v>
+        <v>4</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3140,22 +3407,24 @@
         <v>18</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>39.322908</v>
+        <v>39.322777</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I88" s="0" t="s">
-        <v>105</v>
+        <v>4</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3169,22 +3438,24 @@
         <v>18</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>39.323037</v>
+        <v>39.322908</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I89" s="0" t="s">
-        <v>106</v>
+        <v>4</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3198,22 +3469,24 @@
         <v>18</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>39.323728</v>
+        <v>39.323037</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I90" s="0" t="s">
-        <v>107</v>
+        <v>4</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="0" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3227,22 +3500,24 @@
         <v>18</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>39.32446</v>
+        <v>39.323728</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H91" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I91" s="0" t="s">
-        <v>108</v>
+        <v>4</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3256,22 +3531,24 @@
         <v>18</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>39.325176</v>
+        <v>39.32446</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I92" s="0" t="s">
-        <v>109</v>
+        <v>4</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,22 +3562,24 @@
         <v>18</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>39.325576</v>
+        <v>39.325176</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I93" s="0" t="s">
-        <v>110</v>
+        <v>4</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3314,22 +3593,24 @@
         <v>18</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>39.328434</v>
+        <v>39.325576</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I94" s="0" t="s">
-        <v>111</v>
+        <v>4</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="0" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3343,22 +3624,24 @@
         <v>18</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>39.329121</v>
+        <v>39.328434</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F95" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H95" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I95" s="0" t="s">
-        <v>112</v>
+        <v>4</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,22 +3655,24 @@
         <v>18</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>39.329797</v>
+        <v>39.329121</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I96" s="0" t="s">
-        <v>113</v>
+        <v>4</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3401,22 +3686,24 @@
         <v>18</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>39.331249</v>
+        <v>39.329797</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I97" s="0" t="s">
-        <v>114</v>
+        <v>4</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3430,22 +3717,24 @@
         <v>18</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>39.331425</v>
+        <v>39.331249</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I98" s="0" t="s">
-        <v>115</v>
+        <v>4</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3459,22 +3748,24 @@
         <v>18</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>39.331592</v>
+        <v>39.331425</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I99" s="0" t="s">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I99" s="3"/>
+      <c r="J99" s="3"/>
+      <c r="K99" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3488,22 +3779,24 @@
         <v>18</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>39.33192</v>
+        <v>39.331592</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I100" s="0" t="s">
-        <v>117</v>
+        <v>4</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3517,22 +3810,24 @@
         <v>18</v>
       </c>
       <c r="D101" s="0" t="n">
-        <v>39.332488</v>
+        <v>39.33192</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I101" s="0" t="s">
-        <v>118</v>
+        <v>4</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,22 +3841,24 @@
         <v>18</v>
       </c>
       <c r="D102" s="0" t="n">
-        <v>39.332848</v>
+        <v>39.332488</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H102" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I102" s="0" t="s">
-        <v>119</v>
+        <v>4</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,22 +3872,24 @@
         <v>18</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>39.333202</v>
+        <v>39.332848</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I103" s="0" t="s">
-        <v>120</v>
+        <v>4</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3604,22 +3903,24 @@
         <v>18</v>
       </c>
       <c r="D104" s="0" t="n">
-        <v>39.334364</v>
+        <v>39.333202</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F104" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I104" s="0" t="s">
-        <v>121</v>
+        <v>4</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="0" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3633,22 +3934,24 @@
         <v>18</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>39.33506</v>
+        <v>39.334364</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F105" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H105" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I105" s="0" t="s">
-        <v>122</v>
+        <v>4</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I105" s="3"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3662,22 +3965,24 @@
         <v>18</v>
       </c>
       <c r="D106" s="0" t="n">
-        <v>39.33576</v>
+        <v>39.33506</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F106" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I106" s="0" t="s">
-        <v>123</v>
+        <v>4</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,21 +3996,23 @@
         <v>18</v>
       </c>
       <c r="D107" s="0" t="n">
-        <v>39.332688</v>
+        <v>39.33576</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F107" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I107" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H107" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I107" s="3"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="0" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3720,21 +4027,23 @@
         <v>18</v>
       </c>
       <c r="D108" s="0" t="n">
-        <v>39.323853</v>
+        <v>39.332688</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H108" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H108" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I108" s="0" t="s">
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="0" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3749,21 +4058,24 @@
         <v>18</v>
       </c>
       <c r="D109" s="0" t="n">
-        <v>39.316613</v>
+        <v>39.323853</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F109" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H109" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="I109" s="0" t="s">
+      <c r="I109" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K109" s="0" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3778,22 +4090,24 @@
         <v>18</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>39.317614</v>
+        <v>39.316613</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I110" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H110" s="3" t="s">
         <v>130</v>
+      </c>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3807,22 +4121,24 @@
         <v>18</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>39.326761</v>
+        <v>39.317614</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I111" s="0" t="s">
-        <v>131</v>
+        <v>4</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I111" s="3"/>
+      <c r="J111" s="3"/>
+      <c r="K111" s="0" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3836,22 +4152,24 @@
         <v>18</v>
       </c>
       <c r="D112" s="0" t="n">
-        <v>39.330444</v>
+        <v>39.326761</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F112" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H112" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I112" s="0" t="s">
-        <v>132</v>
+        <v>4</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,22 +4183,55 @@
         <v>18</v>
       </c>
       <c r="D113" s="0" t="n">
+        <v>39.330444</v>
+      </c>
+      <c r="E113" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F113" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G113" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I113" s="3"/>
+      <c r="J113" s="3"/>
+      <c r="K113" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="n">
+        <v>43486</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D114" s="0" t="n">
         <v>39.326015</v>
       </c>
-      <c r="E113" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="F113" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="G113" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H113" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I113" s="0" t="s">
-        <v>134</v>
+      <c r="E114" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F114" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G114" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I114" s="3"/>
+      <c r="J114" s="3"/>
+      <c r="K114" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>